<commit_message>
Create mean_ES summary page for raw_desc_comp report
</commit_message>
<xml_diff>
--- a/CODE/MISC/CROSS-FORM-FRACTIONAL-SAMPLES/OUTPUT-FILES/RAW-DESC-COMP/all-forms-raw-desc-full-60perc-comp.xlsx
+++ b/CODE/MISC/CROSS-FORM-FRACTIONAL-SAMPLES/OUTPUT-FILES/RAW-DESC-COMP/all-forms-raw-desc-full-60perc-comp.xlsx
@@ -7,17 +7,18 @@
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="IT-49-Home" sheetId="1" r:id="rId1"/>
-    <sheet name="IT-1030-Home" sheetId="2" r:id="rId2"/>
-    <sheet name="Preschool-25-Home" sheetId="3" r:id="rId3"/>
-    <sheet name="Preschool-25-School" sheetId="4" r:id="rId4"/>
-    <sheet name="Child-512-Home" sheetId="5" r:id="rId5"/>
-    <sheet name="Child-512-School" sheetId="6" r:id="rId6"/>
-    <sheet name="Teen-1221-Home" sheetId="7" r:id="rId7"/>
-    <sheet name="Teen-1221-School" sheetId="8" r:id="rId8"/>
-    <sheet name="Teen-1221-Self" sheetId="9" r:id="rId9"/>
-    <sheet name="Adult-Self" sheetId="10" r:id="rId10"/>
-    <sheet name="Adult-Other" sheetId="11" r:id="rId11"/>
+    <sheet name="mean_ES" sheetId="1" r:id="rId1"/>
+    <sheet name="IT-49-Home" sheetId="2" r:id="rId2"/>
+    <sheet name="IT-1030-Home" sheetId="3" r:id="rId3"/>
+    <sheet name="Preschool-25-Home" sheetId="4" r:id="rId4"/>
+    <sheet name="Preschool-25-School" sheetId="5" r:id="rId5"/>
+    <sheet name="Child-512-Home" sheetId="6" r:id="rId6"/>
+    <sheet name="Child-512-School" sheetId="7" r:id="rId7"/>
+    <sheet name="Teen-1221-Home" sheetId="8" r:id="rId8"/>
+    <sheet name="Teen-1221-School" sheetId="9" r:id="rId9"/>
+    <sheet name="Teen-1221-Self" sheetId="10" r:id="rId10"/>
+    <sheet name="Adult-Self" sheetId="11" r:id="rId11"/>
+    <sheet name="Adult-Other" sheetId="12" r:id="rId12"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -361,7 +362,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -375,37 +376,7 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>n_full</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>mean_full</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>sd_full</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>n_60perc</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>mean_60perc</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>sd_60perc</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>ES</t>
+          <t>mean_ES</t>
         </is>
       </c>
     </row>
@@ -416,25 +387,7 @@
         </is>
       </c>
       <c r="B2">
-        <v>266</v>
-      </c>
-      <c r="C2">
-        <v>90.038</v>
-      </c>
-      <c r="D2">
-        <v>13.513</v>
-      </c>
-      <c r="E2">
-        <v>204</v>
-      </c>
-      <c r="F2">
-        <v>89.696</v>
-      </c>
-      <c r="G2">
-        <v>13.481</v>
-      </c>
-      <c r="H2">
-        <v>0.025</v>
+        <v>0.026</v>
       </c>
     </row>
     <row r="3">
@@ -444,25 +397,7 @@
         </is>
       </c>
       <c r="B3">
-        <v>266</v>
-      </c>
-      <c r="C3">
-        <v>15.244</v>
-      </c>
-      <c r="D3">
-        <v>4.515</v>
-      </c>
-      <c r="E3">
-        <v>204</v>
-      </c>
-      <c r="F3">
-        <v>14.873</v>
-      </c>
-      <c r="G3">
-        <v>4.342</v>
-      </c>
-      <c r="H3">
-        <v>0.08400000000000001</v>
+        <v>0.026</v>
       </c>
     </row>
     <row r="4">
@@ -472,25 +407,7 @@
         </is>
       </c>
       <c r="B4">
-        <v>266</v>
-      </c>
-      <c r="C4">
-        <v>20.256</v>
-      </c>
-      <c r="D4">
-        <v>4.485</v>
-      </c>
-      <c r="E4">
-        <v>204</v>
-      </c>
-      <c r="F4">
-        <v>20.353</v>
-      </c>
-      <c r="G4">
-        <v>4.691</v>
-      </c>
-      <c r="H4">
-        <v>0.021</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="5">
@@ -500,25 +417,7 @@
         </is>
       </c>
       <c r="B5">
-        <v>266</v>
-      </c>
-      <c r="C5">
-        <v>14.41</v>
-      </c>
-      <c r="D5">
-        <v>2.981</v>
-      </c>
-      <c r="E5">
-        <v>204</v>
-      </c>
-      <c r="F5">
-        <v>14.319</v>
-      </c>
-      <c r="G5">
-        <v>2.973</v>
-      </c>
-      <c r="H5">
-        <v>0.031</v>
+        <v>0.024</v>
       </c>
     </row>
     <row r="6">
@@ -528,25 +427,7 @@
         </is>
       </c>
       <c r="B6">
-        <v>266</v>
-      </c>
-      <c r="C6">
-        <v>14.579</v>
-      </c>
-      <c r="D6">
-        <v>2.926</v>
-      </c>
-      <c r="E6">
-        <v>204</v>
-      </c>
-      <c r="F6">
-        <v>14.426</v>
-      </c>
-      <c r="G6">
-        <v>2.924</v>
-      </c>
-      <c r="H6">
-        <v>0.052</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="7">
@@ -556,25 +437,7 @@
         </is>
       </c>
       <c r="B7">
-        <v>266</v>
-      </c>
-      <c r="C7">
-        <v>11.891</v>
-      </c>
-      <c r="D7">
-        <v>2.556</v>
-      </c>
-      <c r="E7">
-        <v>204</v>
-      </c>
-      <c r="F7">
-        <v>11.892</v>
-      </c>
-      <c r="G7">
-        <v>2.603</v>
-      </c>
-      <c r="H7">
-        <v>0</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="8">
@@ -584,25 +447,7 @@
         </is>
       </c>
       <c r="B8">
-        <v>266</v>
-      </c>
-      <c r="C8">
-        <v>14.695</v>
-      </c>
-      <c r="D8">
-        <v>3.241</v>
-      </c>
-      <c r="E8">
-        <v>204</v>
-      </c>
-      <c r="F8">
-        <v>14.706</v>
-      </c>
-      <c r="G8">
-        <v>3.282</v>
-      </c>
-      <c r="H8">
-        <v>0.003</v>
+        <v>0.023</v>
       </c>
     </row>
     <row r="9">
@@ -612,25 +457,7 @@
         </is>
       </c>
       <c r="B9">
-        <v>266</v>
-      </c>
-      <c r="C9">
-        <v>14.207</v>
-      </c>
-      <c r="D9">
-        <v>3.233</v>
-      </c>
-      <c r="E9">
-        <v>204</v>
-      </c>
-      <c r="F9">
-        <v>14</v>
-      </c>
-      <c r="G9">
-        <v>3.125</v>
-      </c>
-      <c r="H9">
-        <v>0.065</v>
+        <v>0.026</v>
       </c>
     </row>
     <row r="10">
@@ -640,25 +467,7 @@
         </is>
       </c>
       <c r="B10">
-        <v>266</v>
-      </c>
-      <c r="C10">
-        <v>16.605</v>
-      </c>
-      <c r="D10">
-        <v>5.947</v>
-      </c>
-      <c r="E10">
-        <v>204</v>
-      </c>
-      <c r="F10">
-        <v>16.123</v>
-      </c>
-      <c r="G10">
-        <v>5.757</v>
-      </c>
-      <c r="H10">
-        <v>0.082</v>
+        <v>0.021</v>
       </c>
     </row>
   </sheetData>
@@ -723,25 +532,25 @@
         </is>
       </c>
       <c r="B2">
-        <v>711</v>
+        <v>957</v>
       </c>
       <c r="C2">
-        <v>99.79000000000001</v>
+        <v>95.22</v>
       </c>
       <c r="D2">
-        <v>21.921</v>
+        <v>24.028</v>
       </c>
       <c r="E2">
-        <v>442</v>
+        <v>665</v>
       </c>
       <c r="F2">
-        <v>99.681</v>
+        <v>94.83199999999999</v>
       </c>
       <c r="G2">
-        <v>21.839</v>
+        <v>23.908</v>
       </c>
       <c r="H2">
-        <v>0.005</v>
+        <v>0.016</v>
       </c>
     </row>
     <row r="3">
@@ -751,25 +560,25 @@
         </is>
       </c>
       <c r="B3">
-        <v>711</v>
+        <v>957</v>
       </c>
       <c r="C3">
-        <v>18.163</v>
+        <v>17.526</v>
       </c>
       <c r="D3">
-        <v>4.397</v>
+        <v>4.257</v>
       </c>
       <c r="E3">
-        <v>442</v>
+        <v>665</v>
       </c>
       <c r="F3">
-        <v>18.247</v>
+        <v>17.806</v>
       </c>
       <c r="G3">
-        <v>4.338</v>
+        <v>4.346</v>
       </c>
       <c r="H3">
-        <v>0.019</v>
+        <v>0.065</v>
       </c>
     </row>
     <row r="4">
@@ -779,25 +588,25 @@
         </is>
       </c>
       <c r="B4">
-        <v>711</v>
+        <v>957</v>
       </c>
       <c r="C4">
-        <v>15.948</v>
+        <v>16.598</v>
       </c>
       <c r="D4">
-        <v>4.371</v>
+        <v>5.057</v>
       </c>
       <c r="E4">
-        <v>442</v>
+        <v>665</v>
       </c>
       <c r="F4">
-        <v>15.937</v>
+        <v>16.438</v>
       </c>
       <c r="G4">
-        <v>4.293</v>
+        <v>5.025</v>
       </c>
       <c r="H4">
-        <v>0.003</v>
+        <v>0.032</v>
       </c>
     </row>
     <row r="5">
@@ -807,25 +616,25 @@
         </is>
       </c>
       <c r="B5">
-        <v>711</v>
+        <v>957</v>
       </c>
       <c r="C5">
-        <v>18.629</v>
+        <v>16.853</v>
       </c>
       <c r="D5">
-        <v>5.281</v>
+        <v>5.188</v>
       </c>
       <c r="E5">
-        <v>442</v>
+        <v>665</v>
       </c>
       <c r="F5">
-        <v>18.502</v>
+        <v>16.895</v>
       </c>
       <c r="G5">
-        <v>5.255</v>
+        <v>5.141</v>
       </c>
       <c r="H5">
-        <v>0.024</v>
+        <v>0.008</v>
       </c>
     </row>
     <row r="6">
@@ -835,25 +644,25 @@
         </is>
       </c>
       <c r="B6">
-        <v>711</v>
+        <v>957</v>
       </c>
       <c r="C6">
-        <v>17.395</v>
+        <v>15.41</v>
       </c>
       <c r="D6">
-        <v>4.421</v>
+        <v>4.184</v>
       </c>
       <c r="E6">
-        <v>442</v>
+        <v>665</v>
       </c>
       <c r="F6">
-        <v>17.425</v>
+        <v>15.32</v>
       </c>
       <c r="G6">
-        <v>4.388</v>
+        <v>4.078</v>
       </c>
       <c r="H6">
-        <v>0.007</v>
+        <v>0.022</v>
       </c>
     </row>
     <row r="7">
@@ -863,25 +672,25 @@
         </is>
       </c>
       <c r="B7">
-        <v>711</v>
+        <v>957</v>
       </c>
       <c r="C7">
-        <v>17.439</v>
+        <v>17.208</v>
       </c>
       <c r="D7">
-        <v>4.457</v>
+        <v>5.067</v>
       </c>
       <c r="E7">
-        <v>442</v>
+        <v>665</v>
       </c>
       <c r="F7">
-        <v>17.511</v>
+        <v>17.086</v>
       </c>
       <c r="G7">
-        <v>4.351</v>
+        <v>4.937</v>
       </c>
       <c r="H7">
-        <v>0.016</v>
+        <v>0.024</v>
       </c>
     </row>
     <row r="8">
@@ -891,25 +700,25 @@
         </is>
       </c>
       <c r="B8">
-        <v>711</v>
+        <v>957</v>
       </c>
       <c r="C8">
-        <v>13.977</v>
+        <v>15.103</v>
       </c>
       <c r="D8">
-        <v>3.983</v>
+        <v>4.615</v>
       </c>
       <c r="E8">
-        <v>442</v>
+        <v>665</v>
       </c>
       <c r="F8">
-        <v>14.029</v>
+        <v>15.069</v>
       </c>
       <c r="G8">
-        <v>3.968</v>
+        <v>4.736</v>
       </c>
       <c r="H8">
-        <v>0.013</v>
+        <v>0.007</v>
       </c>
     </row>
     <row r="9">
@@ -919,25 +728,25 @@
         </is>
       </c>
       <c r="B9">
-        <v>711</v>
+        <v>957</v>
       </c>
       <c r="C9">
-        <v>16.402</v>
+        <v>14.049</v>
       </c>
       <c r="D9">
-        <v>4.805</v>
+        <v>4.253</v>
       </c>
       <c r="E9">
-        <v>442</v>
+        <v>665</v>
       </c>
       <c r="F9">
-        <v>16.276</v>
+        <v>14.024</v>
       </c>
       <c r="G9">
-        <v>4.834</v>
+        <v>4.249</v>
       </c>
       <c r="H9">
-        <v>0.026</v>
+        <v>0.006</v>
       </c>
     </row>
     <row r="10">
@@ -947,25 +756,25 @@
         </is>
       </c>
       <c r="B10">
-        <v>711</v>
+        <v>957</v>
       </c>
       <c r="C10">
-        <v>16.599</v>
+        <v>16.242</v>
       </c>
       <c r="D10">
-        <v>4.898</v>
+        <v>4.968</v>
       </c>
       <c r="E10">
-        <v>442</v>
+        <v>665</v>
       </c>
       <c r="F10">
-        <v>16.59</v>
+        <v>16.265</v>
       </c>
       <c r="G10">
-        <v>4.917</v>
+        <v>5.001</v>
       </c>
       <c r="H10">
-        <v>0.002</v>
+        <v>0.004</v>
       </c>
     </row>
   </sheetData>
@@ -1030,6 +839,313 @@
         </is>
       </c>
       <c r="B2">
+        <v>711</v>
+      </c>
+      <c r="C2">
+        <v>99.79000000000001</v>
+      </c>
+      <c r="D2">
+        <v>21.921</v>
+      </c>
+      <c r="E2">
+        <v>442</v>
+      </c>
+      <c r="F2">
+        <v>99.681</v>
+      </c>
+      <c r="G2">
+        <v>21.839</v>
+      </c>
+      <c r="H2">
+        <v>0.005</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>SOC_raw</t>
+        </is>
+      </c>
+      <c r="B3">
+        <v>711</v>
+      </c>
+      <c r="C3">
+        <v>18.163</v>
+      </c>
+      <c r="D3">
+        <v>4.397</v>
+      </c>
+      <c r="E3">
+        <v>442</v>
+      </c>
+      <c r="F3">
+        <v>18.247</v>
+      </c>
+      <c r="G3">
+        <v>4.338</v>
+      </c>
+      <c r="H3">
+        <v>0.019</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>VIS_raw</t>
+        </is>
+      </c>
+      <c r="B4">
+        <v>711</v>
+      </c>
+      <c r="C4">
+        <v>15.948</v>
+      </c>
+      <c r="D4">
+        <v>4.371</v>
+      </c>
+      <c r="E4">
+        <v>442</v>
+      </c>
+      <c r="F4">
+        <v>15.937</v>
+      </c>
+      <c r="G4">
+        <v>4.293</v>
+      </c>
+      <c r="H4">
+        <v>0.003</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>HEA_raw</t>
+        </is>
+      </c>
+      <c r="B5">
+        <v>711</v>
+      </c>
+      <c r="C5">
+        <v>18.629</v>
+      </c>
+      <c r="D5">
+        <v>5.281</v>
+      </c>
+      <c r="E5">
+        <v>442</v>
+      </c>
+      <c r="F5">
+        <v>18.502</v>
+      </c>
+      <c r="G5">
+        <v>5.255</v>
+      </c>
+      <c r="H5">
+        <v>0.024</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>TOU_raw</t>
+        </is>
+      </c>
+      <c r="B6">
+        <v>711</v>
+      </c>
+      <c r="C6">
+        <v>17.395</v>
+      </c>
+      <c r="D6">
+        <v>4.421</v>
+      </c>
+      <c r="E6">
+        <v>442</v>
+      </c>
+      <c r="F6">
+        <v>17.425</v>
+      </c>
+      <c r="G6">
+        <v>4.388</v>
+      </c>
+      <c r="H6">
+        <v>0.007</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>TS_raw</t>
+        </is>
+      </c>
+      <c r="B7">
+        <v>711</v>
+      </c>
+      <c r="C7">
+        <v>17.439</v>
+      </c>
+      <c r="D7">
+        <v>4.457</v>
+      </c>
+      <c r="E7">
+        <v>442</v>
+      </c>
+      <c r="F7">
+        <v>17.511</v>
+      </c>
+      <c r="G7">
+        <v>4.351</v>
+      </c>
+      <c r="H7">
+        <v>0.016</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>BOD_raw</t>
+        </is>
+      </c>
+      <c r="B8">
+        <v>711</v>
+      </c>
+      <c r="C8">
+        <v>13.977</v>
+      </c>
+      <c r="D8">
+        <v>3.983</v>
+      </c>
+      <c r="E8">
+        <v>442</v>
+      </c>
+      <c r="F8">
+        <v>14.029</v>
+      </c>
+      <c r="G8">
+        <v>3.968</v>
+      </c>
+      <c r="H8">
+        <v>0.013</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>BAL_raw</t>
+        </is>
+      </c>
+      <c r="B9">
+        <v>711</v>
+      </c>
+      <c r="C9">
+        <v>16.402</v>
+      </c>
+      <c r="D9">
+        <v>4.805</v>
+      </c>
+      <c r="E9">
+        <v>442</v>
+      </c>
+      <c r="F9">
+        <v>16.276</v>
+      </c>
+      <c r="G9">
+        <v>4.834</v>
+      </c>
+      <c r="H9">
+        <v>0.026</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>PLA_raw</t>
+        </is>
+      </c>
+      <c r="B10">
+        <v>711</v>
+      </c>
+      <c r="C10">
+        <v>16.599</v>
+      </c>
+      <c r="D10">
+        <v>4.898</v>
+      </c>
+      <c r="E10">
+        <v>442</v>
+      </c>
+      <c r="F10">
+        <v>16.59</v>
+      </c>
+      <c r="G10">
+        <v>4.917</v>
+      </c>
+      <c r="H10">
+        <v>0.002</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:H10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" s="1" customFormat="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>scale</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>n_full</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>mean_full</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>sd_full</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>n_60perc</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>mean_60perc</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>sd_60perc</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>ES</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>TOT_raw</t>
+        </is>
+      </c>
+      <c r="B2">
         <v>604</v>
       </c>
       <c r="C2">
@@ -1337,25 +1453,25 @@
         </is>
       </c>
       <c r="B2">
-        <v>422</v>
+        <v>266</v>
       </c>
       <c r="C2">
-        <v>88.36</v>
+        <v>90.038</v>
       </c>
       <c r="D2">
-        <v>15.664</v>
+        <v>13.513</v>
       </c>
       <c r="E2">
-        <v>365</v>
+        <v>204</v>
       </c>
       <c r="F2">
-        <v>88.56999999999999</v>
+        <v>89.696</v>
       </c>
       <c r="G2">
-        <v>15.894</v>
+        <v>13.481</v>
       </c>
       <c r="H2">
-        <v>0.013</v>
+        <v>0.025</v>
       </c>
     </row>
     <row r="3">
@@ -1365,25 +1481,25 @@
         </is>
       </c>
       <c r="B3">
-        <v>422</v>
+        <v>266</v>
       </c>
       <c r="C3">
-        <v>16.344</v>
+        <v>15.244</v>
       </c>
       <c r="D3">
-        <v>4.541</v>
+        <v>4.515</v>
       </c>
       <c r="E3">
-        <v>365</v>
+        <v>204</v>
       </c>
       <c r="F3">
-        <v>16.43</v>
+        <v>14.873</v>
       </c>
       <c r="G3">
-        <v>4.593</v>
+        <v>4.342</v>
       </c>
       <c r="H3">
-        <v>0.019</v>
+        <v>0.08400000000000001</v>
       </c>
     </row>
     <row r="4">
@@ -1393,25 +1509,25 @@
         </is>
       </c>
       <c r="B4">
-        <v>422</v>
+        <v>266</v>
       </c>
       <c r="C4">
-        <v>15.86</v>
+        <v>20.256</v>
       </c>
       <c r="D4">
-        <v>3.664</v>
+        <v>4.485</v>
       </c>
       <c r="E4">
-        <v>365</v>
+        <v>204</v>
       </c>
       <c r="F4">
-        <v>16</v>
+        <v>20.353</v>
       </c>
       <c r="G4">
-        <v>3.717</v>
+        <v>4.691</v>
       </c>
       <c r="H4">
-        <v>0.038</v>
+        <v>0.021</v>
       </c>
     </row>
     <row r="5">
@@ -1421,25 +1537,25 @@
         </is>
       </c>
       <c r="B5">
-        <v>422</v>
+        <v>266</v>
       </c>
       <c r="C5">
-        <v>15.379</v>
+        <v>14.41</v>
       </c>
       <c r="D5">
-        <v>3.592</v>
+        <v>2.981</v>
       </c>
       <c r="E5">
-        <v>365</v>
+        <v>204</v>
       </c>
       <c r="F5">
-        <v>15.411</v>
+        <v>14.319</v>
       </c>
       <c r="G5">
-        <v>3.6</v>
+        <v>2.973</v>
       </c>
       <c r="H5">
-        <v>0.008999999999999999</v>
+        <v>0.031</v>
       </c>
     </row>
     <row r="6">
@@ -1449,25 +1565,25 @@
         </is>
       </c>
       <c r="B6">
-        <v>422</v>
+        <v>266</v>
       </c>
       <c r="C6">
-        <v>14.595</v>
+        <v>14.579</v>
       </c>
       <c r="D6">
-        <v>3.204</v>
+        <v>2.926</v>
       </c>
       <c r="E6">
-        <v>365</v>
+        <v>204</v>
       </c>
       <c r="F6">
-        <v>14.605</v>
+        <v>14.426</v>
       </c>
       <c r="G6">
-        <v>3.19</v>
+        <v>2.924</v>
       </c>
       <c r="H6">
-        <v>0.003</v>
+        <v>0.052</v>
       </c>
     </row>
     <row r="7">
@@ -1477,25 +1593,25 @@
         </is>
       </c>
       <c r="B7">
-        <v>422</v>
+        <v>266</v>
       </c>
       <c r="C7">
-        <v>13.164</v>
+        <v>11.891</v>
       </c>
       <c r="D7">
-        <v>3.084</v>
+        <v>2.556</v>
       </c>
       <c r="E7">
-        <v>365</v>
+        <v>204</v>
       </c>
       <c r="F7">
-        <v>13.09</v>
+        <v>11.892</v>
       </c>
       <c r="G7">
-        <v>3.084</v>
+        <v>2.603</v>
       </c>
       <c r="H7">
-        <v>0.024</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8">
@@ -1505,25 +1621,25 @@
         </is>
       </c>
       <c r="B8">
-        <v>422</v>
+        <v>266</v>
       </c>
       <c r="C8">
-        <v>15.374</v>
+        <v>14.695</v>
       </c>
       <c r="D8">
-        <v>3.579</v>
+        <v>3.241</v>
       </c>
       <c r="E8">
-        <v>365</v>
+        <v>204</v>
       </c>
       <c r="F8">
-        <v>15.441</v>
+        <v>14.706</v>
       </c>
       <c r="G8">
-        <v>3.664</v>
+        <v>3.282</v>
       </c>
       <c r="H8">
-        <v>0.018</v>
+        <v>0.003</v>
       </c>
     </row>
     <row r="9">
@@ -1533,25 +1649,25 @@
         </is>
       </c>
       <c r="B9">
-        <v>422</v>
+        <v>266</v>
       </c>
       <c r="C9">
-        <v>13.988</v>
+        <v>14.207</v>
       </c>
       <c r="D9">
-        <v>3.313</v>
+        <v>3.233</v>
       </c>
       <c r="E9">
-        <v>365</v>
+        <v>204</v>
       </c>
       <c r="F9">
-        <v>14.022</v>
+        <v>14</v>
       </c>
       <c r="G9">
-        <v>3.43</v>
+        <v>3.125</v>
       </c>
       <c r="H9">
-        <v>0.01</v>
+        <v>0.065</v>
       </c>
     </row>
     <row r="10">
@@ -1561,25 +1677,25 @@
         </is>
       </c>
       <c r="B10">
-        <v>421</v>
+        <v>266</v>
       </c>
       <c r="C10">
-        <v>13.387</v>
+        <v>16.605</v>
       </c>
       <c r="D10">
-        <v>4.277</v>
+        <v>5.947</v>
       </c>
       <c r="E10">
-        <v>364</v>
+        <v>204</v>
       </c>
       <c r="F10">
-        <v>13.434</v>
+        <v>16.123</v>
       </c>
       <c r="G10">
-        <v>4.319</v>
+        <v>5.757</v>
       </c>
       <c r="H10">
-        <v>0.011</v>
+        <v>0.082</v>
       </c>
     </row>
   </sheetData>
@@ -1644,25 +1760,25 @@
         </is>
       </c>
       <c r="B2">
-        <v>520</v>
+        <v>422</v>
       </c>
       <c r="C2">
-        <v>88.842</v>
+        <v>88.36</v>
       </c>
       <c r="D2">
-        <v>21.912</v>
+        <v>15.664</v>
       </c>
       <c r="E2">
-        <v>340</v>
+        <v>365</v>
       </c>
       <c r="F2">
-        <v>90.685</v>
+        <v>88.56999999999999</v>
       </c>
       <c r="G2">
-        <v>22.476</v>
+        <v>15.894</v>
       </c>
       <c r="H2">
-        <v>0.083</v>
+        <v>0.013</v>
       </c>
     </row>
     <row r="3">
@@ -1672,25 +1788,25 @@
         </is>
       </c>
       <c r="B3">
-        <v>520</v>
+        <v>422</v>
       </c>
       <c r="C3">
-        <v>19.517</v>
+        <v>16.344</v>
       </c>
       <c r="D3">
-        <v>5.491</v>
+        <v>4.541</v>
       </c>
       <c r="E3">
-        <v>340</v>
+        <v>365</v>
       </c>
       <c r="F3">
-        <v>19.424</v>
+        <v>16.43</v>
       </c>
       <c r="G3">
-        <v>5.378</v>
+        <v>4.593</v>
       </c>
       <c r="H3">
-        <v>0.017</v>
+        <v>0.019</v>
       </c>
     </row>
     <row r="4">
@@ -1700,25 +1816,25 @@
         </is>
       </c>
       <c r="B4">
-        <v>520</v>
+        <v>422</v>
       </c>
       <c r="C4">
-        <v>15.935</v>
+        <v>15.86</v>
       </c>
       <c r="D4">
-        <v>4.717</v>
+        <v>3.664</v>
       </c>
       <c r="E4">
-        <v>340</v>
+        <v>365</v>
       </c>
       <c r="F4">
-        <v>16.282</v>
+        <v>16</v>
       </c>
       <c r="G4">
-        <v>4.723</v>
+        <v>3.717</v>
       </c>
       <c r="H4">
-        <v>0.074</v>
+        <v>0.038</v>
       </c>
     </row>
     <row r="5">
@@ -1728,25 +1844,25 @@
         </is>
       </c>
       <c r="B5">
-        <v>520</v>
+        <v>422</v>
       </c>
       <c r="C5">
-        <v>15.515</v>
+        <v>15.379</v>
       </c>
       <c r="D5">
-        <v>5.082</v>
+        <v>3.592</v>
       </c>
       <c r="E5">
-        <v>340</v>
+        <v>365</v>
       </c>
       <c r="F5">
-        <v>15.844</v>
+        <v>15.411</v>
       </c>
       <c r="G5">
-        <v>5.261</v>
+        <v>3.6</v>
       </c>
       <c r="H5">
-        <v>0.064</v>
+        <v>0.008999999999999999</v>
       </c>
     </row>
     <row r="6">
@@ -1756,25 +1872,25 @@
         </is>
       </c>
       <c r="B6">
-        <v>520</v>
+        <v>422</v>
       </c>
       <c r="C6">
-        <v>14.479</v>
+        <v>14.595</v>
       </c>
       <c r="D6">
-        <v>4.272</v>
+        <v>3.204</v>
       </c>
       <c r="E6">
-        <v>340</v>
+        <v>365</v>
       </c>
       <c r="F6">
-        <v>14.876</v>
+        <v>14.605</v>
       </c>
       <c r="G6">
-        <v>4.557</v>
+        <v>3.19</v>
       </c>
       <c r="H6">
-        <v>0.091</v>
+        <v>0.003</v>
       </c>
     </row>
     <row r="7">
@@ -1784,25 +1900,25 @@
         </is>
       </c>
       <c r="B7">
-        <v>520</v>
+        <v>422</v>
       </c>
       <c r="C7">
-        <v>14.065</v>
+        <v>13.164</v>
       </c>
       <c r="D7">
-        <v>3.991</v>
+        <v>3.084</v>
       </c>
       <c r="E7">
-        <v>340</v>
+        <v>365</v>
       </c>
       <c r="F7">
-        <v>14.365</v>
+        <v>13.09</v>
       </c>
       <c r="G7">
-        <v>4.087</v>
+        <v>3.084</v>
       </c>
       <c r="H7">
-        <v>0.074</v>
+        <v>0.024</v>
       </c>
     </row>
     <row r="8">
@@ -1812,25 +1928,25 @@
         </is>
       </c>
       <c r="B8">
-        <v>520</v>
+        <v>422</v>
       </c>
       <c r="C8">
-        <v>15.848</v>
+        <v>15.374</v>
       </c>
       <c r="D8">
-        <v>4.958</v>
+        <v>3.579</v>
       </c>
       <c r="E8">
-        <v>340</v>
+        <v>365</v>
       </c>
       <c r="F8">
-        <v>16.147</v>
+        <v>15.441</v>
       </c>
       <c r="G8">
-        <v>5.101</v>
+        <v>3.664</v>
       </c>
       <c r="H8">
-        <v>0.06</v>
+        <v>0.018</v>
       </c>
     </row>
     <row r="9">
@@ -1840,25 +1956,25 @@
         </is>
       </c>
       <c r="B9">
-        <v>520</v>
+        <v>422</v>
       </c>
       <c r="C9">
-        <v>13</v>
+        <v>13.988</v>
       </c>
       <c r="D9">
-        <v>3.438</v>
+        <v>3.313</v>
       </c>
       <c r="E9">
-        <v>340</v>
+        <v>365</v>
       </c>
       <c r="F9">
-        <v>13.171</v>
+        <v>14.022</v>
       </c>
       <c r="G9">
-        <v>3.52</v>
+        <v>3.43</v>
       </c>
       <c r="H9">
-        <v>0.049</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="10">
@@ -1868,25 +1984,25 @@
         </is>
       </c>
       <c r="B10">
-        <v>520</v>
+        <v>421</v>
       </c>
       <c r="C10">
-        <v>15.192</v>
+        <v>13.387</v>
       </c>
       <c r="D10">
-        <v>4.628</v>
+        <v>4.277</v>
       </c>
       <c r="E10">
-        <v>340</v>
+        <v>364</v>
       </c>
       <c r="F10">
-        <v>15.376</v>
+        <v>13.434</v>
       </c>
       <c r="G10">
-        <v>4.55</v>
+        <v>4.319</v>
       </c>
       <c r="H10">
-        <v>0.04</v>
+        <v>0.011</v>
       </c>
     </row>
   </sheetData>
@@ -1951,25 +2067,25 @@
         </is>
       </c>
       <c r="B2">
-        <v>539</v>
+        <v>520</v>
       </c>
       <c r="C2">
-        <v>77.306</v>
+        <v>88.842</v>
       </c>
       <c r="D2">
-        <v>19.018</v>
+        <v>21.912</v>
       </c>
       <c r="E2">
-        <v>333</v>
+        <v>340</v>
       </c>
       <c r="F2">
-        <v>78.345</v>
+        <v>90.685</v>
       </c>
       <c r="G2">
-        <v>20.254</v>
+        <v>22.476</v>
       </c>
       <c r="H2">
-        <v>0.053</v>
+        <v>0.083</v>
       </c>
     </row>
     <row r="3">
@@ -1979,22 +2095,22 @@
         </is>
       </c>
       <c r="B3">
-        <v>539</v>
+        <v>520</v>
       </c>
       <c r="C3">
-        <v>18.583</v>
+        <v>19.517</v>
       </c>
       <c r="D3">
-        <v>5.939</v>
+        <v>5.491</v>
       </c>
       <c r="E3">
-        <v>333</v>
+        <v>340</v>
       </c>
       <c r="F3">
-        <v>18.682</v>
+        <v>19.424</v>
       </c>
       <c r="G3">
-        <v>5.824</v>
+        <v>5.378</v>
       </c>
       <c r="H3">
         <v>0.017</v>
@@ -2007,25 +2123,25 @@
         </is>
       </c>
       <c r="B4">
-        <v>539</v>
+        <v>520</v>
       </c>
       <c r="C4">
-        <v>13.688</v>
+        <v>15.935</v>
       </c>
       <c r="D4">
-        <v>3.863</v>
+        <v>4.717</v>
       </c>
       <c r="E4">
-        <v>333</v>
+        <v>340</v>
       </c>
       <c r="F4">
-        <v>13.874</v>
+        <v>16.282</v>
       </c>
       <c r="G4">
-        <v>4.041</v>
+        <v>4.723</v>
       </c>
       <c r="H4">
-        <v>0.047</v>
+        <v>0.074</v>
       </c>
     </row>
     <row r="5">
@@ -2035,25 +2151,25 @@
         </is>
       </c>
       <c r="B5">
-        <v>539</v>
+        <v>520</v>
       </c>
       <c r="C5">
-        <v>13.74</v>
+        <v>15.515</v>
       </c>
       <c r="D5">
-        <v>4.086</v>
+        <v>5.082</v>
       </c>
       <c r="E5">
-        <v>333</v>
+        <v>340</v>
       </c>
       <c r="F5">
-        <v>13.91</v>
+        <v>15.844</v>
       </c>
       <c r="G5">
-        <v>4.24</v>
+        <v>5.261</v>
       </c>
       <c r="H5">
-        <v>0.041</v>
+        <v>0.064</v>
       </c>
     </row>
     <row r="6">
@@ -2063,25 +2179,25 @@
         </is>
       </c>
       <c r="B6">
-        <v>539</v>
+        <v>520</v>
       </c>
       <c r="C6">
-        <v>12.855</v>
+        <v>14.479</v>
       </c>
       <c r="D6">
-        <v>3.604</v>
+        <v>4.272</v>
       </c>
       <c r="E6">
-        <v>333</v>
+        <v>340</v>
       </c>
       <c r="F6">
-        <v>13.042</v>
+        <v>14.876</v>
       </c>
       <c r="G6">
-        <v>3.718</v>
+        <v>4.557</v>
       </c>
       <c r="H6">
-        <v>0.051</v>
+        <v>0.091</v>
       </c>
     </row>
     <row r="7">
@@ -2091,25 +2207,25 @@
         </is>
       </c>
       <c r="B7">
-        <v>539</v>
+        <v>520</v>
       </c>
       <c r="C7">
-        <v>11.863</v>
+        <v>14.065</v>
       </c>
       <c r="D7">
-        <v>3.134</v>
+        <v>3.991</v>
       </c>
       <c r="E7">
-        <v>333</v>
+        <v>340</v>
       </c>
       <c r="F7">
-        <v>12.06</v>
+        <v>14.365</v>
       </c>
       <c r="G7">
-        <v>3.463</v>
+        <v>4.087</v>
       </c>
       <c r="H7">
-        <v>0.06</v>
+        <v>0.074</v>
       </c>
     </row>
     <row r="8">
@@ -2119,25 +2235,25 @@
         </is>
       </c>
       <c r="B8">
-        <v>539</v>
+        <v>520</v>
       </c>
       <c r="C8">
-        <v>12.944</v>
+        <v>15.848</v>
       </c>
       <c r="D8">
-        <v>4.03</v>
+        <v>4.958</v>
       </c>
       <c r="E8">
-        <v>333</v>
+        <v>340</v>
       </c>
       <c r="F8">
-        <v>13.141</v>
+        <v>16.147</v>
       </c>
       <c r="G8">
-        <v>4.248</v>
+        <v>5.101</v>
       </c>
       <c r="H8">
-        <v>0.048</v>
+        <v>0.06</v>
       </c>
     </row>
     <row r="9">
@@ -2147,25 +2263,25 @@
         </is>
       </c>
       <c r="B9">
-        <v>539</v>
+        <v>520</v>
       </c>
       <c r="C9">
-        <v>12.215</v>
+        <v>13</v>
       </c>
       <c r="D9">
-        <v>3.239</v>
+        <v>3.438</v>
       </c>
       <c r="E9">
-        <v>333</v>
+        <v>340</v>
       </c>
       <c r="F9">
-        <v>12.318</v>
+        <v>13.171</v>
       </c>
       <c r="G9">
-        <v>3.425</v>
+        <v>3.52</v>
       </c>
       <c r="H9">
-        <v>0.031</v>
+        <v>0.049</v>
       </c>
     </row>
     <row r="10">
@@ -2175,25 +2291,25 @@
         </is>
       </c>
       <c r="B10">
-        <v>539</v>
+        <v>520</v>
       </c>
       <c r="C10">
-        <v>14.609</v>
+        <v>15.192</v>
       </c>
       <c r="D10">
-        <v>4.702</v>
+        <v>4.628</v>
       </c>
       <c r="E10">
-        <v>333</v>
+        <v>340</v>
       </c>
       <c r="F10">
-        <v>14.658</v>
+        <v>15.376</v>
       </c>
       <c r="G10">
-        <v>4.758</v>
+        <v>4.55</v>
       </c>
       <c r="H10">
-        <v>0.01</v>
+        <v>0.04</v>
       </c>
     </row>
   </sheetData>
@@ -2258,25 +2374,25 @@
         </is>
       </c>
       <c r="B2">
-        <v>875</v>
+        <v>539</v>
       </c>
       <c r="C2">
-        <v>79.77800000000001</v>
+        <v>77.306</v>
       </c>
       <c r="D2">
-        <v>17.285</v>
+        <v>19.018</v>
       </c>
       <c r="E2">
-        <v>601</v>
+        <v>333</v>
       </c>
       <c r="F2">
-        <v>79.506</v>
+        <v>78.345</v>
       </c>
       <c r="G2">
-        <v>16.983</v>
+        <v>20.254</v>
       </c>
       <c r="H2">
-        <v>0.016</v>
+        <v>0.053</v>
       </c>
     </row>
     <row r="3">
@@ -2286,25 +2402,25 @@
         </is>
       </c>
       <c r="B3">
-        <v>875</v>
+        <v>539</v>
       </c>
       <c r="C3">
-        <v>17.174</v>
+        <v>18.583</v>
       </c>
       <c r="D3">
-        <v>5.495</v>
+        <v>5.939</v>
       </c>
       <c r="E3">
-        <v>601</v>
+        <v>333</v>
       </c>
       <c r="F3">
-        <v>17.161</v>
+        <v>18.682</v>
       </c>
       <c r="G3">
-        <v>5.479</v>
+        <v>5.824</v>
       </c>
       <c r="H3">
-        <v>0.002</v>
+        <v>0.017</v>
       </c>
     </row>
     <row r="4">
@@ -2314,25 +2430,25 @@
         </is>
       </c>
       <c r="B4">
-        <v>875</v>
+        <v>539</v>
       </c>
       <c r="C4">
-        <v>13.175</v>
+        <v>13.688</v>
       </c>
       <c r="D4">
-        <v>3.386</v>
+        <v>3.863</v>
       </c>
       <c r="E4">
-        <v>601</v>
+        <v>333</v>
       </c>
       <c r="F4">
-        <v>13.128</v>
+        <v>13.874</v>
       </c>
       <c r="G4">
-        <v>3.343</v>
+        <v>4.041</v>
       </c>
       <c r="H4">
-        <v>0.014</v>
+        <v>0.047</v>
       </c>
     </row>
     <row r="5">
@@ -2342,25 +2458,25 @@
         </is>
       </c>
       <c r="B5">
-        <v>875</v>
+        <v>539</v>
       </c>
       <c r="C5">
-        <v>12.991</v>
+        <v>13.74</v>
       </c>
       <c r="D5">
-        <v>4.009</v>
+        <v>4.086</v>
       </c>
       <c r="E5">
-        <v>601</v>
+        <v>333</v>
       </c>
       <c r="F5">
-        <v>13.038</v>
+        <v>13.91</v>
       </c>
       <c r="G5">
-        <v>4.021</v>
+        <v>4.24</v>
       </c>
       <c r="H5">
-        <v>0.012</v>
+        <v>0.041</v>
       </c>
     </row>
     <row r="6">
@@ -2370,25 +2486,25 @@
         </is>
       </c>
       <c r="B6">
-        <v>875</v>
+        <v>539</v>
       </c>
       <c r="C6">
-        <v>13.584</v>
+        <v>12.855</v>
       </c>
       <c r="D6">
-        <v>3.43</v>
+        <v>3.604</v>
       </c>
       <c r="E6">
-        <v>601</v>
+        <v>333</v>
       </c>
       <c r="F6">
-        <v>13.496</v>
+        <v>13.042</v>
       </c>
       <c r="G6">
-        <v>3.292</v>
+        <v>3.718</v>
       </c>
       <c r="H6">
-        <v>0.026</v>
+        <v>0.051</v>
       </c>
     </row>
     <row r="7">
@@ -2398,25 +2514,25 @@
         </is>
       </c>
       <c r="B7">
-        <v>875</v>
+        <v>539</v>
       </c>
       <c r="C7">
-        <v>14.138</v>
+        <v>11.863</v>
       </c>
       <c r="D7">
-        <v>3.846</v>
+        <v>3.134</v>
       </c>
       <c r="E7">
-        <v>601</v>
+        <v>333</v>
       </c>
       <c r="F7">
-        <v>14.07</v>
+        <v>12.06</v>
       </c>
       <c r="G7">
-        <v>3.738</v>
+        <v>3.463</v>
       </c>
       <c r="H7">
-        <v>0.018</v>
+        <v>0.06</v>
       </c>
     </row>
     <row r="8">
@@ -2426,25 +2542,25 @@
         </is>
       </c>
       <c r="B8">
-        <v>875</v>
+        <v>539</v>
       </c>
       <c r="C8">
-        <v>13.746</v>
+        <v>12.944</v>
       </c>
       <c r="D8">
-        <v>3.902</v>
+        <v>4.03</v>
       </c>
       <c r="E8">
-        <v>601</v>
+        <v>333</v>
       </c>
       <c r="F8">
-        <v>13.709</v>
+        <v>13.141</v>
       </c>
       <c r="G8">
-        <v>3.938</v>
+        <v>4.248</v>
       </c>
       <c r="H8">
-        <v>0.01</v>
+        <v>0.048</v>
       </c>
     </row>
     <row r="9">
@@ -2454,25 +2570,25 @@
         </is>
       </c>
       <c r="B9">
-        <v>875</v>
+        <v>539</v>
       </c>
       <c r="C9">
-        <v>12.144</v>
+        <v>12.215</v>
       </c>
       <c r="D9">
-        <v>2.827</v>
+        <v>3.239</v>
       </c>
       <c r="E9">
-        <v>601</v>
+        <v>333</v>
       </c>
       <c r="F9">
-        <v>12.065</v>
+        <v>12.318</v>
       </c>
       <c r="G9">
-        <v>2.782</v>
+        <v>3.425</v>
       </c>
       <c r="H9">
-        <v>0.028</v>
+        <v>0.031</v>
       </c>
     </row>
     <row r="10">
@@ -2482,25 +2598,25 @@
         </is>
       </c>
       <c r="B10">
-        <v>875</v>
+        <v>539</v>
       </c>
       <c r="C10">
-        <v>14.062</v>
+        <v>14.609</v>
       </c>
       <c r="D10">
-        <v>4.332</v>
+        <v>4.702</v>
       </c>
       <c r="E10">
-        <v>601</v>
+        <v>333</v>
       </c>
       <c r="F10">
-        <v>14.005</v>
+        <v>14.658</v>
       </c>
       <c r="G10">
-        <v>4.27</v>
+        <v>4.758</v>
       </c>
       <c r="H10">
-        <v>0.013</v>
+        <v>0.01</v>
       </c>
     </row>
   </sheetData>
@@ -2565,25 +2681,25 @@
         </is>
       </c>
       <c r="B2">
-        <v>617</v>
+        <v>875</v>
       </c>
       <c r="C2">
-        <v>73.52500000000001</v>
+        <v>79.77800000000001</v>
       </c>
       <c r="D2">
-        <v>15.94</v>
+        <v>17.285</v>
       </c>
       <c r="E2">
-        <v>390</v>
+        <v>601</v>
       </c>
       <c r="F2">
-        <v>73.205</v>
+        <v>79.506</v>
       </c>
       <c r="G2">
-        <v>15.714</v>
+        <v>16.983</v>
       </c>
       <c r="H2">
-        <v>0.02</v>
+        <v>0.016</v>
       </c>
     </row>
     <row r="3">
@@ -2593,25 +2709,25 @@
         </is>
       </c>
       <c r="B3">
-        <v>617</v>
+        <v>875</v>
       </c>
       <c r="C3">
-        <v>15.418</v>
+        <v>17.174</v>
       </c>
       <c r="D3">
-        <v>5.433</v>
+        <v>5.495</v>
       </c>
       <c r="E3">
-        <v>390</v>
+        <v>601</v>
       </c>
       <c r="F3">
-        <v>15.351</v>
+        <v>17.161</v>
       </c>
       <c r="G3">
-        <v>5.429</v>
+        <v>5.479</v>
       </c>
       <c r="H3">
-        <v>0.012</v>
+        <v>0.002</v>
       </c>
     </row>
     <row r="4">
@@ -2621,25 +2737,25 @@
         </is>
       </c>
       <c r="B4">
-        <v>617</v>
+        <v>875</v>
       </c>
       <c r="C4">
-        <v>13.603</v>
+        <v>13.175</v>
       </c>
       <c r="D4">
-        <v>3.553</v>
+        <v>3.386</v>
       </c>
       <c r="E4">
-        <v>390</v>
+        <v>601</v>
       </c>
       <c r="F4">
-        <v>13.495</v>
+        <v>13.128</v>
       </c>
       <c r="G4">
-        <v>3.513</v>
+        <v>3.343</v>
       </c>
       <c r="H4">
-        <v>0.031</v>
+        <v>0.014</v>
       </c>
     </row>
     <row r="5">
@@ -2649,25 +2765,25 @@
         </is>
       </c>
       <c r="B5">
-        <v>617</v>
+        <v>875</v>
       </c>
       <c r="C5">
-        <v>13.112</v>
+        <v>12.991</v>
       </c>
       <c r="D5">
-        <v>3.621</v>
+        <v>4.009</v>
       </c>
       <c r="E5">
-        <v>390</v>
+        <v>601</v>
       </c>
       <c r="F5">
-        <v>13.077</v>
+        <v>13.038</v>
       </c>
       <c r="G5">
-        <v>3.688</v>
+        <v>4.021</v>
       </c>
       <c r="H5">
-        <v>0.01</v>
+        <v>0.012</v>
       </c>
     </row>
     <row r="6">
@@ -2677,25 +2793,25 @@
         </is>
       </c>
       <c r="B6">
-        <v>617</v>
+        <v>875</v>
       </c>
       <c r="C6">
-        <v>11.429</v>
+        <v>13.584</v>
       </c>
       <c r="D6">
-        <v>2.455</v>
+        <v>3.43</v>
       </c>
       <c r="E6">
-        <v>390</v>
+        <v>601</v>
       </c>
       <c r="F6">
-        <v>11.395</v>
+        <v>13.496</v>
       </c>
       <c r="G6">
-        <v>2.407</v>
+        <v>3.292</v>
       </c>
       <c r="H6">
-        <v>0.014</v>
+        <v>0.026</v>
       </c>
     </row>
     <row r="7">
@@ -2705,25 +2821,25 @@
         </is>
       </c>
       <c r="B7">
-        <v>617</v>
+        <v>875</v>
       </c>
       <c r="C7">
-        <v>11.222</v>
+        <v>14.138</v>
       </c>
       <c r="D7">
-        <v>2.518</v>
+        <v>3.846</v>
       </c>
       <c r="E7">
-        <v>390</v>
+        <v>601</v>
       </c>
       <c r="F7">
-        <v>11.174</v>
+        <v>14.07</v>
       </c>
       <c r="G7">
-        <v>2.311</v>
+        <v>3.738</v>
       </c>
       <c r="H7">
-        <v>0.02</v>
+        <v>0.018</v>
       </c>
     </row>
     <row r="8">
@@ -2733,25 +2849,25 @@
         </is>
       </c>
       <c r="B8">
-        <v>617</v>
+        <v>875</v>
       </c>
       <c r="C8">
-        <v>11.88</v>
+        <v>13.746</v>
       </c>
       <c r="D8">
-        <v>3.294</v>
+        <v>3.902</v>
       </c>
       <c r="E8">
-        <v>390</v>
+        <v>601</v>
       </c>
       <c r="F8">
-        <v>11.797</v>
+        <v>13.709</v>
       </c>
       <c r="G8">
-        <v>3.113</v>
+        <v>3.938</v>
       </c>
       <c r="H8">
-        <v>0.026</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="9">
@@ -2761,25 +2877,25 @@
         </is>
       </c>
       <c r="B9">
-        <v>617</v>
+        <v>875</v>
       </c>
       <c r="C9">
-        <v>12.279</v>
+        <v>12.144</v>
       </c>
       <c r="D9">
-        <v>3.187</v>
+        <v>2.827</v>
       </c>
       <c r="E9">
-        <v>390</v>
+        <v>601</v>
       </c>
       <c r="F9">
-        <v>12.267</v>
+        <v>12.065</v>
       </c>
       <c r="G9">
-        <v>3.162</v>
+        <v>2.782</v>
       </c>
       <c r="H9">
-        <v>0.004</v>
+        <v>0.028</v>
       </c>
     </row>
     <row r="10">
@@ -2789,25 +2905,25 @@
         </is>
       </c>
       <c r="B10">
-        <v>617</v>
+        <v>875</v>
       </c>
       <c r="C10">
-        <v>14.418</v>
+        <v>14.062</v>
       </c>
       <c r="D10">
-        <v>5.058</v>
+        <v>4.332</v>
       </c>
       <c r="E10">
-        <v>390</v>
+        <v>601</v>
       </c>
       <c r="F10">
-        <v>14.408</v>
+        <v>14.005</v>
       </c>
       <c r="G10">
-        <v>5.022</v>
+        <v>4.27</v>
       </c>
       <c r="H10">
-        <v>0.002</v>
+        <v>0.013</v>
       </c>
     </row>
   </sheetData>
@@ -2872,25 +2988,25 @@
         </is>
       </c>
       <c r="B2">
-        <v>1014</v>
+        <v>617</v>
       </c>
       <c r="C2">
-        <v>78.925</v>
+        <v>73.52500000000001</v>
       </c>
       <c r="D2">
-        <v>21.141</v>
+        <v>15.94</v>
       </c>
       <c r="E2">
-        <v>662</v>
+        <v>390</v>
       </c>
       <c r="F2">
-        <v>79.258</v>
+        <v>73.205</v>
       </c>
       <c r="G2">
-        <v>21.412</v>
+        <v>15.714</v>
       </c>
       <c r="H2">
-        <v>0.016</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="3">
@@ -2900,25 +3016,25 @@
         </is>
       </c>
       <c r="B3">
-        <v>1014</v>
+        <v>617</v>
       </c>
       <c r="C3">
-        <v>17.441</v>
+        <v>15.418</v>
       </c>
       <c r="D3">
-        <v>4.87</v>
+        <v>5.433</v>
       </c>
       <c r="E3">
-        <v>662</v>
+        <v>390</v>
       </c>
       <c r="F3">
-        <v>17.579</v>
+        <v>15.351</v>
       </c>
       <c r="G3">
-        <v>4.922</v>
+        <v>5.429</v>
       </c>
       <c r="H3">
-        <v>0.028</v>
+        <v>0.012</v>
       </c>
     </row>
     <row r="4">
@@ -2928,25 +3044,25 @@
         </is>
       </c>
       <c r="B4">
-        <v>1014</v>
+        <v>617</v>
       </c>
       <c r="C4">
-        <v>13.228</v>
+        <v>13.603</v>
       </c>
       <c r="D4">
-        <v>4.045</v>
+        <v>3.553</v>
       </c>
       <c r="E4">
-        <v>662</v>
+        <v>390</v>
       </c>
       <c r="F4">
-        <v>13.216</v>
+        <v>13.495</v>
       </c>
       <c r="G4">
-        <v>4.015</v>
+        <v>3.513</v>
       </c>
       <c r="H4">
-        <v>0.003</v>
+        <v>0.031</v>
       </c>
     </row>
     <row r="5">
@@ -2956,25 +3072,25 @@
         </is>
       </c>
       <c r="B5">
-        <v>1014</v>
+        <v>617</v>
       </c>
       <c r="C5">
-        <v>13.158</v>
+        <v>13.112</v>
       </c>
       <c r="D5">
-        <v>4.168</v>
+        <v>3.621</v>
       </c>
       <c r="E5">
-        <v>662</v>
+        <v>390</v>
       </c>
       <c r="F5">
-        <v>13.228</v>
+        <v>13.077</v>
       </c>
       <c r="G5">
-        <v>4.141</v>
+        <v>3.688</v>
       </c>
       <c r="H5">
-        <v>0.017</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="6">
@@ -2984,25 +3100,25 @@
         </is>
       </c>
       <c r="B6">
-        <v>1014</v>
+        <v>617</v>
       </c>
       <c r="C6">
-        <v>12.86</v>
+        <v>11.429</v>
       </c>
       <c r="D6">
-        <v>3.971</v>
+        <v>2.455</v>
       </c>
       <c r="E6">
-        <v>662</v>
+        <v>390</v>
       </c>
       <c r="F6">
-        <v>12.905</v>
+        <v>11.395</v>
       </c>
       <c r="G6">
-        <v>3.994</v>
+        <v>2.407</v>
       </c>
       <c r="H6">
-        <v>0.011</v>
+        <v>0.014</v>
       </c>
     </row>
     <row r="7">
@@ -3012,25 +3128,25 @@
         </is>
       </c>
       <c r="B7">
-        <v>1014</v>
+        <v>617</v>
       </c>
       <c r="C7">
-        <v>14.641</v>
+        <v>11.222</v>
       </c>
       <c r="D7">
-        <v>4.531</v>
+        <v>2.518</v>
       </c>
       <c r="E7">
-        <v>662</v>
+        <v>390</v>
       </c>
       <c r="F7">
-        <v>14.776</v>
+        <v>11.174</v>
       </c>
       <c r="G7">
-        <v>4.535</v>
+        <v>2.311</v>
       </c>
       <c r="H7">
-        <v>0.03</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="8">
@@ -3040,25 +3156,25 @@
         </is>
       </c>
       <c r="B8">
-        <v>1014</v>
+        <v>617</v>
       </c>
       <c r="C8">
-        <v>12.959</v>
+        <v>11.88</v>
       </c>
       <c r="D8">
-        <v>4.122</v>
+        <v>3.294</v>
       </c>
       <c r="E8">
-        <v>662</v>
+        <v>390</v>
       </c>
       <c r="F8">
-        <v>13.003</v>
+        <v>11.797</v>
       </c>
       <c r="G8">
-        <v>4.202</v>
+        <v>3.113</v>
       </c>
       <c r="H8">
-        <v>0.011</v>
+        <v>0.026</v>
       </c>
     </row>
     <row r="9">
@@ -3068,25 +3184,25 @@
         </is>
       </c>
       <c r="B9">
-        <v>1014</v>
+        <v>617</v>
       </c>
       <c r="C9">
-        <v>12.08</v>
+        <v>12.279</v>
       </c>
       <c r="D9">
-        <v>3.818</v>
+        <v>3.187</v>
       </c>
       <c r="E9">
-        <v>662</v>
+        <v>390</v>
       </c>
       <c r="F9">
-        <v>12.13</v>
+        <v>12.267</v>
       </c>
       <c r="G9">
-        <v>3.939</v>
+        <v>3.162</v>
       </c>
       <c r="H9">
-        <v>0.013</v>
+        <v>0.004</v>
       </c>
     </row>
     <row r="10">
@@ -3096,25 +3212,25 @@
         </is>
       </c>
       <c r="B10">
-        <v>1014</v>
+        <v>617</v>
       </c>
       <c r="C10">
-        <v>14.425</v>
+        <v>14.418</v>
       </c>
       <c r="D10">
-        <v>5.246</v>
+        <v>5.058</v>
       </c>
       <c r="E10">
-        <v>662</v>
+        <v>390</v>
       </c>
       <c r="F10">
-        <v>14.53</v>
+        <v>14.408</v>
       </c>
       <c r="G10">
-        <v>5.516</v>
+        <v>5.022</v>
       </c>
       <c r="H10">
-        <v>0.02</v>
+        <v>0.002</v>
       </c>
     </row>
   </sheetData>
@@ -3179,25 +3295,25 @@
         </is>
       </c>
       <c r="B2">
-        <v>645</v>
+        <v>1014</v>
       </c>
       <c r="C2">
-        <v>69.051</v>
+        <v>78.925</v>
       </c>
       <c r="D2">
-        <v>19.327</v>
+        <v>21.141</v>
       </c>
       <c r="E2">
-        <v>406</v>
+        <v>662</v>
       </c>
       <c r="F2">
-        <v>69.943</v>
+        <v>79.258</v>
       </c>
       <c r="G2">
-        <v>21.779</v>
+        <v>21.412</v>
       </c>
       <c r="H2">
-        <v>0.044</v>
+        <v>0.016</v>
       </c>
     </row>
     <row r="3">
@@ -3207,25 +3323,25 @@
         </is>
       </c>
       <c r="B3">
-        <v>645</v>
+        <v>1014</v>
       </c>
       <c r="C3">
-        <v>17.448</v>
+        <v>17.441</v>
       </c>
       <c r="D3">
-        <v>5.642</v>
+        <v>4.87</v>
       </c>
       <c r="E3">
-        <v>406</v>
+        <v>662</v>
       </c>
       <c r="F3">
-        <v>17.35</v>
+        <v>17.579</v>
       </c>
       <c r="G3">
-        <v>5.746</v>
+        <v>4.922</v>
       </c>
       <c r="H3">
-        <v>0.017</v>
+        <v>0.028</v>
       </c>
     </row>
     <row r="4">
@@ -3235,25 +3351,25 @@
         </is>
       </c>
       <c r="B4">
-        <v>645</v>
+        <v>1014</v>
       </c>
       <c r="C4">
-        <v>11.633</v>
+        <v>13.228</v>
       </c>
       <c r="D4">
-        <v>3.581</v>
+        <v>4.045</v>
       </c>
       <c r="E4">
-        <v>406</v>
+        <v>662</v>
       </c>
       <c r="F4">
-        <v>11.82</v>
+        <v>13.216</v>
       </c>
       <c r="G4">
-        <v>4.047</v>
+        <v>4.015</v>
       </c>
       <c r="H4">
-        <v>0.05</v>
+        <v>0.003</v>
       </c>
     </row>
     <row r="5">
@@ -3263,25 +3379,25 @@
         </is>
       </c>
       <c r="B5">
-        <v>645</v>
+        <v>1014</v>
       </c>
       <c r="C5">
-        <v>11.971</v>
+        <v>13.158</v>
       </c>
       <c r="D5">
-        <v>3.855</v>
+        <v>4.168</v>
       </c>
       <c r="E5">
-        <v>406</v>
+        <v>662</v>
       </c>
       <c r="F5">
-        <v>12.126</v>
+        <v>13.228</v>
       </c>
       <c r="G5">
-        <v>4.275</v>
+        <v>4.141</v>
       </c>
       <c r="H5">
-        <v>0.039</v>
+        <v>0.017</v>
       </c>
     </row>
     <row r="6">
@@ -3291,25 +3407,25 @@
         </is>
       </c>
       <c r="B6">
-        <v>645</v>
+        <v>1014</v>
       </c>
       <c r="C6">
-        <v>11.15</v>
+        <v>12.86</v>
       </c>
       <c r="D6">
-        <v>3.068</v>
+        <v>3.971</v>
       </c>
       <c r="E6">
-        <v>406</v>
+        <v>662</v>
       </c>
       <c r="F6">
-        <v>11.261</v>
+        <v>12.905</v>
       </c>
       <c r="G6">
-        <v>3.44</v>
+        <v>3.994</v>
       </c>
       <c r="H6">
-        <v>0.034</v>
+        <v>0.011</v>
       </c>
     </row>
     <row r="7">
@@ -3319,25 +3435,25 @@
         </is>
       </c>
       <c r="B7">
-        <v>645</v>
+        <v>1014</v>
       </c>
       <c r="C7">
-        <v>11.544</v>
+        <v>14.641</v>
       </c>
       <c r="D7">
-        <v>3.51</v>
+        <v>4.531</v>
       </c>
       <c r="E7">
-        <v>406</v>
+        <v>662</v>
       </c>
       <c r="F7">
-        <v>11.707</v>
+        <v>14.776</v>
       </c>
       <c r="G7">
-        <v>3.872</v>
+        <v>4.535</v>
       </c>
       <c r="H7">
-        <v>0.045</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="8">
@@ -3347,25 +3463,25 @@
         </is>
       </c>
       <c r="B8">
-        <v>645</v>
+        <v>1014</v>
       </c>
       <c r="C8">
-        <v>11.375</v>
+        <v>12.959</v>
       </c>
       <c r="D8">
-        <v>3.393</v>
+        <v>4.122</v>
       </c>
       <c r="E8">
-        <v>406</v>
+        <v>662</v>
       </c>
       <c r="F8">
-        <v>11.522</v>
+        <v>13.003</v>
       </c>
       <c r="G8">
-        <v>3.813</v>
+        <v>4.202</v>
       </c>
       <c r="H8">
-        <v>0.041</v>
+        <v>0.011</v>
       </c>
     </row>
     <row r="9">
@@ -3375,25 +3491,25 @@
         </is>
       </c>
       <c r="B9">
-        <v>645</v>
+        <v>1014</v>
       </c>
       <c r="C9">
-        <v>11.378</v>
+        <v>12.08</v>
       </c>
       <c r="D9">
-        <v>3.457</v>
+        <v>3.818</v>
       </c>
       <c r="E9">
-        <v>406</v>
+        <v>662</v>
       </c>
       <c r="F9">
-        <v>11.507</v>
+        <v>12.13</v>
       </c>
       <c r="G9">
-        <v>3.862</v>
+        <v>3.939</v>
       </c>
       <c r="H9">
-        <v>0.036</v>
+        <v>0.013</v>
       </c>
     </row>
     <row r="10">
@@ -3403,25 +3519,25 @@
         </is>
       </c>
       <c r="B10">
-        <v>645</v>
+        <v>1014</v>
       </c>
       <c r="C10">
-        <v>13.994</v>
+        <v>14.425</v>
       </c>
       <c r="D10">
-        <v>4.979</v>
+        <v>5.246</v>
       </c>
       <c r="E10">
-        <v>406</v>
+        <v>662</v>
       </c>
       <c r="F10">
-        <v>14.207</v>
+        <v>14.53</v>
       </c>
       <c r="G10">
-        <v>5.241</v>
+        <v>5.516</v>
       </c>
       <c r="H10">
-        <v>0.042</v>
+        <v>0.02</v>
       </c>
     </row>
   </sheetData>
@@ -3486,25 +3602,25 @@
         </is>
       </c>
       <c r="B2">
-        <v>957</v>
+        <v>645</v>
       </c>
       <c r="C2">
-        <v>95.22</v>
+        <v>69.051</v>
       </c>
       <c r="D2">
-        <v>24.028</v>
+        <v>19.327</v>
       </c>
       <c r="E2">
-        <v>665</v>
+        <v>406</v>
       </c>
       <c r="F2">
-        <v>94.83199999999999</v>
+        <v>69.943</v>
       </c>
       <c r="G2">
-        <v>23.908</v>
+        <v>21.779</v>
       </c>
       <c r="H2">
-        <v>0.016</v>
+        <v>0.044</v>
       </c>
     </row>
     <row r="3">
@@ -3514,25 +3630,25 @@
         </is>
       </c>
       <c r="B3">
-        <v>957</v>
+        <v>645</v>
       </c>
       <c r="C3">
-        <v>17.526</v>
+        <v>17.448</v>
       </c>
       <c r="D3">
-        <v>4.257</v>
+        <v>5.642</v>
       </c>
       <c r="E3">
-        <v>665</v>
+        <v>406</v>
       </c>
       <c r="F3">
-        <v>17.806</v>
+        <v>17.35</v>
       </c>
       <c r="G3">
-        <v>4.346</v>
+        <v>5.746</v>
       </c>
       <c r="H3">
-        <v>0.065</v>
+        <v>0.017</v>
       </c>
     </row>
     <row r="4">
@@ -3542,25 +3658,25 @@
         </is>
       </c>
       <c r="B4">
-        <v>957</v>
+        <v>645</v>
       </c>
       <c r="C4">
-        <v>16.598</v>
+        <v>11.633</v>
       </c>
       <c r="D4">
-        <v>5.057</v>
+        <v>3.581</v>
       </c>
       <c r="E4">
-        <v>665</v>
+        <v>406</v>
       </c>
       <c r="F4">
-        <v>16.438</v>
+        <v>11.82</v>
       </c>
       <c r="G4">
-        <v>5.025</v>
+        <v>4.047</v>
       </c>
       <c r="H4">
-        <v>0.032</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="5">
@@ -3570,25 +3686,25 @@
         </is>
       </c>
       <c r="B5">
-        <v>957</v>
+        <v>645</v>
       </c>
       <c r="C5">
-        <v>16.853</v>
+        <v>11.971</v>
       </c>
       <c r="D5">
-        <v>5.188</v>
+        <v>3.855</v>
       </c>
       <c r="E5">
-        <v>665</v>
+        <v>406</v>
       </c>
       <c r="F5">
-        <v>16.895</v>
+        <v>12.126</v>
       </c>
       <c r="G5">
-        <v>5.141</v>
+        <v>4.275</v>
       </c>
       <c r="H5">
-        <v>0.008</v>
+        <v>0.039</v>
       </c>
     </row>
     <row r="6">
@@ -3598,25 +3714,25 @@
         </is>
       </c>
       <c r="B6">
-        <v>957</v>
+        <v>645</v>
       </c>
       <c r="C6">
-        <v>15.41</v>
+        <v>11.15</v>
       </c>
       <c r="D6">
-        <v>4.184</v>
+        <v>3.068</v>
       </c>
       <c r="E6">
-        <v>665</v>
+        <v>406</v>
       </c>
       <c r="F6">
-        <v>15.32</v>
+        <v>11.261</v>
       </c>
       <c r="G6">
-        <v>4.078</v>
+        <v>3.44</v>
       </c>
       <c r="H6">
-        <v>0.022</v>
+        <v>0.034</v>
       </c>
     </row>
     <row r="7">
@@ -3626,25 +3742,25 @@
         </is>
       </c>
       <c r="B7">
-        <v>957</v>
+        <v>645</v>
       </c>
       <c r="C7">
-        <v>17.208</v>
+        <v>11.544</v>
       </c>
       <c r="D7">
-        <v>5.067</v>
+        <v>3.51</v>
       </c>
       <c r="E7">
-        <v>665</v>
+        <v>406</v>
       </c>
       <c r="F7">
-        <v>17.086</v>
+        <v>11.707</v>
       </c>
       <c r="G7">
-        <v>4.937</v>
+        <v>3.872</v>
       </c>
       <c r="H7">
-        <v>0.024</v>
+        <v>0.045</v>
       </c>
     </row>
     <row r="8">
@@ -3654,25 +3770,25 @@
         </is>
       </c>
       <c r="B8">
-        <v>957</v>
+        <v>645</v>
       </c>
       <c r="C8">
-        <v>15.103</v>
+        <v>11.375</v>
       </c>
       <c r="D8">
-        <v>4.615</v>
+        <v>3.393</v>
       </c>
       <c r="E8">
-        <v>665</v>
+        <v>406</v>
       </c>
       <c r="F8">
-        <v>15.069</v>
+        <v>11.522</v>
       </c>
       <c r="G8">
-        <v>4.736</v>
+        <v>3.813</v>
       </c>
       <c r="H8">
-        <v>0.007</v>
+        <v>0.041</v>
       </c>
     </row>
     <row r="9">
@@ -3682,25 +3798,25 @@
         </is>
       </c>
       <c r="B9">
-        <v>957</v>
+        <v>645</v>
       </c>
       <c r="C9">
-        <v>14.049</v>
+        <v>11.378</v>
       </c>
       <c r="D9">
-        <v>4.253</v>
+        <v>3.457</v>
       </c>
       <c r="E9">
-        <v>665</v>
+        <v>406</v>
       </c>
       <c r="F9">
-        <v>14.024</v>
+        <v>11.507</v>
       </c>
       <c r="G9">
-        <v>4.249</v>
+        <v>3.862</v>
       </c>
       <c r="H9">
-        <v>0.006</v>
+        <v>0.036</v>
       </c>
     </row>
     <row r="10">
@@ -3710,25 +3826,25 @@
         </is>
       </c>
       <c r="B10">
-        <v>957</v>
+        <v>645</v>
       </c>
       <c r="C10">
-        <v>16.242</v>
+        <v>13.994</v>
       </c>
       <c r="D10">
-        <v>4.968</v>
+        <v>4.979</v>
       </c>
       <c r="E10">
-        <v>665</v>
+        <v>406</v>
       </c>
       <c r="F10">
-        <v>16.265</v>
+        <v>14.207</v>
       </c>
       <c r="G10">
-        <v>5.001</v>
+        <v>5.241</v>
       </c>
       <c r="H10">
-        <v>0.004</v>
+        <v>0.042</v>
       </c>
     </row>
   </sheetData>

</xml_diff>